<commit_message>
grafo salas listo, solo falta AP
</commit_message>
<xml_diff>
--- a/Datos/Salas SJ 2023-07-13.xlsx
+++ b/Datos/Salas SJ 2023-07-13.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\IPre\IPre20232Calendario\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7C65C2-0161-4D31-AB98-0E8C2CADA247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75766D57-5A46-45E2-92E9-0BEAE13900EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="2868" windowWidth="21912" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2082,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A165" sqref="A165:XFD165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2948,171 +2948,171 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="3">
         <v>60</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="3">
         <v>60</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="3">
         <v>80</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="65" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="3">
         <v>80</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="3">
         <v>80</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="3">
         <v>25</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="68" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="3">
         <v>40</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="69" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="3">
         <v>25</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="70" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="3">
         <v>40</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="71" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="3">
         <v>40</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="72" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="3">
         <v>40</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="73" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="3">
         <v>40</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="3" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3284,87 +3284,87 @@
         <v>133</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="3">
         <v>60</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="87" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="3">
         <v>30</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="88" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="3">
         <v>60</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="89" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="3">
         <v>30</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="90" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="3">
         <v>60</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="91" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="3">
         <v>30</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="3" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3382,17 +3382,17 @@
         <v>195</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="93" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="3">
         <v>27</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="3" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3438,17 +3438,17 @@
         <v>195</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="97" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="3">
         <v>24</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="3" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3522,17 +3522,17 @@
         <v>195</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="103" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="3">
         <v>25</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="3" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3872,31 +3872,31 @@
         <v>228</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="128" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C128">
+      <c r="C128" s="3">
         <v>25</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="129" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="3">
         <v>25</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="3" t="s">
         <v>228</v>
       </c>
     </row>
@@ -4390,17 +4390,17 @@
         <v>278</v>
       </c>
     </row>
-    <row r="165" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="4" t="s">
+    <row r="165" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B165" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="C165" s="4">
+      <c r="C165" s="3">
         <v>25</v>
       </c>
-      <c r="D165" s="4" t="s">
+      <c r="D165" s="3" t="s">
         <v>278</v>
       </c>
     </row>

</xml_diff>

<commit_message>
salas funcionando con todo
</commit_message>
<xml_diff>
--- a/Datos/Salas SJ 2023-07-13.xlsx
+++ b/Datos/Salas SJ 2023-07-13.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b60417830953b312/Escritorio/iPre/IPre20232Calendario/Datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\andre\Desktop\IPre\IPre20232Calendario\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FDB327E8-71C4-4904-AA91-8AE16E4B5AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42AB47FB-729A-43F0-91F5-BC1A898A0B13}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EBB69E-163A-4B38-AFB9-2F53C82FC507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21912" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="530">
   <si>
     <t>Location Name</t>
   </si>
@@ -1616,13 +1616,16 @@
     <t>Sala de clases AP604 Edificio de Aulas Las Pataguas</t>
   </si>
   <si>
-    <t>usar</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -2053,10 +2056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:F251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2067,7 +2070,7 @@
     <col min="4" max="4" width="38.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2081,10 +2084,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>528</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2098,10 +2104,13 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2115,10 +2124,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2132,10 +2144,13 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2149,10 +2164,13 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2166,10 +2184,13 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2183,10 +2204,13 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2200,10 +2224,13 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2217,10 +2244,13 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -2234,10 +2264,13 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2251,10 +2284,13 @@
         <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2268,10 +2304,13 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2285,10 +2324,13 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2302,10 +2344,13 @@
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2319,10 +2364,13 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2336,10 +2384,13 @@
         <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2353,10 +2404,13 @@
         <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2370,10 +2424,13 @@
         <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -2387,10 +2444,13 @@
         <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2404,10 +2464,13 @@
         <v>40</v>
       </c>
       <c r="E20" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2421,10 +2484,13 @@
         <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -2438,10 +2504,13 @@
         <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2455,10 +2524,13 @@
         <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2472,10 +2544,13 @@
         <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -2489,10 +2564,13 @@
         <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2506,10 +2584,13 @@
         <v>40</v>
       </c>
       <c r="E26" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -2523,10 +2604,13 @@
         <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -2540,10 +2624,13 @@
         <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -2557,10 +2644,13 @@
         <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -2574,10 +2664,13 @@
         <v>40</v>
       </c>
       <c r="E30" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -2591,10 +2684,13 @@
         <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -2608,10 +2704,13 @@
         <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -2625,10 +2724,13 @@
         <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -2642,10 +2744,13 @@
         <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -2659,10 +2764,13 @@
         <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -2676,10 +2784,13 @@
         <v>40</v>
       </c>
       <c r="E36" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -2693,10 +2804,13 @@
         <v>79</v>
       </c>
       <c r="E37" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>80</v>
       </c>
@@ -2710,10 +2824,13 @@
         <v>79</v>
       </c>
       <c r="E38" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -2727,10 +2844,13 @@
         <v>84</v>
       </c>
       <c r="E39" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -2744,10 +2864,13 @@
         <v>84</v>
       </c>
       <c r="E40" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -2761,10 +2884,13 @@
         <v>84</v>
       </c>
       <c r="E41" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2778,10 +2904,13 @@
         <v>84</v>
       </c>
       <c r="E42" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -2795,10 +2924,13 @@
         <v>84</v>
       </c>
       <c r="E43" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -2812,10 +2944,13 @@
         <v>84</v>
       </c>
       <c r="E44" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -2829,10 +2964,13 @@
         <v>84</v>
       </c>
       <c r="E45" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -2846,10 +2984,13 @@
         <v>84</v>
       </c>
       <c r="E46" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>99</v>
       </c>
@@ -2863,10 +3004,13 @@
         <v>84</v>
       </c>
       <c r="E47" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>101</v>
       </c>
@@ -2880,10 +3024,13 @@
         <v>84</v>
       </c>
       <c r="E48" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -2897,10 +3044,13 @@
         <v>105</v>
       </c>
       <c r="E49" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -2914,10 +3064,13 @@
         <v>105</v>
       </c>
       <c r="E50" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -2931,10 +3084,13 @@
         <v>105</v>
       </c>
       <c r="E51" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -2948,10 +3104,13 @@
         <v>105</v>
       </c>
       <c r="E52" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -2965,10 +3124,13 @@
         <v>105</v>
       </c>
       <c r="E53" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -2982,10 +3144,13 @@
         <v>105</v>
       </c>
       <c r="E54" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>116</v>
       </c>
@@ -2999,10 +3164,13 @@
         <v>105</v>
       </c>
       <c r="E55" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F55">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>118</v>
       </c>
@@ -3016,10 +3184,13 @@
         <v>105</v>
       </c>
       <c r="E56" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>120</v>
       </c>
@@ -3033,10 +3204,13 @@
         <v>105</v>
       </c>
       <c r="E57" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>122</v>
       </c>
@@ -3050,10 +3224,13 @@
         <v>105</v>
       </c>
       <c r="E58" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F58">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>124</v>
       </c>
@@ -3067,10 +3244,13 @@
         <v>105</v>
       </c>
       <c r="E59" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>126</v>
       </c>
@@ -3084,10 +3264,13 @@
         <v>105</v>
       </c>
       <c r="E60" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -3101,10 +3284,10 @@
         <v>130</v>
       </c>
       <c r="E61" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -3118,10 +3301,10 @@
         <v>130</v>
       </c>
       <c r="E62" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>133</v>
       </c>
@@ -3135,10 +3318,10 @@
         <v>130</v>
       </c>
       <c r="E63" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -3152,7 +3335,7 @@
         <v>130</v>
       </c>
       <c r="E64" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3169,7 +3352,7 @@
         <v>130</v>
       </c>
       <c r="E65" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3186,7 +3369,7 @@
         <v>130</v>
       </c>
       <c r="E66" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3203,7 +3386,7 @@
         <v>130</v>
       </c>
       <c r="E67" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3220,7 +3403,7 @@
         <v>130</v>
       </c>
       <c r="E68" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3237,7 +3420,7 @@
         <v>130</v>
       </c>
       <c r="E69" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3254,7 +3437,7 @@
         <v>130</v>
       </c>
       <c r="E70" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3271,7 +3454,7 @@
         <v>130</v>
       </c>
       <c r="E71" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3288,7 +3471,7 @@
         <v>130</v>
       </c>
       <c r="E72" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3305,7 +3488,7 @@
         <v>130</v>
       </c>
       <c r="E73" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3322,7 +3505,7 @@
         <v>130</v>
       </c>
       <c r="E74" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3339,7 +3522,7 @@
         <v>130</v>
       </c>
       <c r="E75" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3356,7 +3539,7 @@
         <v>130</v>
       </c>
       <c r="E76" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3373,7 +3556,7 @@
         <v>130</v>
       </c>
       <c r="E77" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3390,7 +3573,7 @@
         <v>130</v>
       </c>
       <c r="E78" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3407,7 +3590,7 @@
         <v>130</v>
       </c>
       <c r="E79" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3424,10 +3607,10 @@
         <v>130</v>
       </c>
       <c r="E80" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -3441,10 +3624,10 @@
         <v>130</v>
       </c>
       <c r="E81" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -3458,10 +3641,10 @@
         <v>130</v>
       </c>
       <c r="E82" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -3475,10 +3658,10 @@
         <v>130</v>
       </c>
       <c r="E83" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>175</v>
       </c>
@@ -3492,10 +3675,10 @@
         <v>130</v>
       </c>
       <c r="E84" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>177</v>
       </c>
@@ -3509,10 +3692,10 @@
         <v>179</v>
       </c>
       <c r="E85" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>180</v>
       </c>
@@ -3526,10 +3709,10 @@
         <v>179</v>
       </c>
       <c r="E86" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>182</v>
       </c>
@@ -3543,10 +3726,10 @@
         <v>179</v>
       </c>
       <c r="E87" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>184</v>
       </c>
@@ -3560,10 +3743,10 @@
         <v>179</v>
       </c>
       <c r="E88" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>186</v>
       </c>
@@ -3577,10 +3760,10 @@
         <v>179</v>
       </c>
       <c r="E89" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>188</v>
       </c>
@@ -3594,10 +3777,10 @@
         <v>179</v>
       </c>
       <c r="E90" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>190</v>
       </c>
@@ -3611,10 +3794,13 @@
         <v>192</v>
       </c>
       <c r="E91" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F91">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>193</v>
       </c>
@@ -3628,10 +3814,13 @@
         <v>192</v>
       </c>
       <c r="E92" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F92">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>195</v>
       </c>
@@ -3645,10 +3834,13 @@
         <v>192</v>
       </c>
       <c r="E93" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F93">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>197</v>
       </c>
@@ -3662,10 +3854,13 @@
         <v>192</v>
       </c>
       <c r="E94" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F94">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>199</v>
       </c>
@@ -3679,10 +3874,13 @@
         <v>192</v>
       </c>
       <c r="E95" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F95">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>201</v>
       </c>
@@ -3696,10 +3894,13 @@
         <v>192</v>
       </c>
       <c r="E96" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F96">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>203</v>
       </c>
@@ -3713,10 +3914,13 @@
         <v>192</v>
       </c>
       <c r="E97" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>205</v>
       </c>
@@ -3730,10 +3934,13 @@
         <v>192</v>
       </c>
       <c r="E98" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F98">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>207</v>
       </c>
@@ -3747,10 +3954,13 @@
         <v>192</v>
       </c>
       <c r="E99" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F99">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>209</v>
       </c>
@@ -3764,10 +3974,13 @@
         <v>192</v>
       </c>
       <c r="E100" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F100">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>211</v>
       </c>
@@ -3781,10 +3994,13 @@
         <v>192</v>
       </c>
       <c r="E101" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F101">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>213</v>
       </c>
@@ -3798,10 +4014,13 @@
         <v>192</v>
       </c>
       <c r="E102" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F102">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>215</v>
       </c>
@@ -3815,10 +4034,13 @@
         <v>192</v>
       </c>
       <c r="E103" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F103">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>217</v>
       </c>
@@ -3832,10 +4054,13 @@
         <v>192</v>
       </c>
       <c r="E104" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F104">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>219</v>
       </c>
@@ -3849,10 +4074,13 @@
         <v>192</v>
       </c>
       <c r="E105" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F105">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>221</v>
       </c>
@@ -3866,10 +4094,13 @@
         <v>192</v>
       </c>
       <c r="E106" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F106">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>223</v>
       </c>
@@ -3883,10 +4114,13 @@
         <v>225</v>
       </c>
       <c r="E107" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F107">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>226</v>
       </c>
@@ -3900,10 +4134,13 @@
         <v>225</v>
       </c>
       <c r="E108" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F108">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>228</v>
       </c>
@@ -3917,10 +4154,13 @@
         <v>225</v>
       </c>
       <c r="E109" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F109">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>230</v>
       </c>
@@ -3934,10 +4174,13 @@
         <v>225</v>
       </c>
       <c r="E110" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F110">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>232</v>
       </c>
@@ -3951,10 +4194,13 @@
         <v>225</v>
       </c>
       <c r="E111" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F111">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>234</v>
       </c>
@@ -3968,10 +4214,13 @@
         <v>225</v>
       </c>
       <c r="E112" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F112">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>236</v>
       </c>
@@ -3985,10 +4234,13 @@
         <v>225</v>
       </c>
       <c r="E113" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F113">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>238</v>
       </c>
@@ -4002,10 +4254,13 @@
         <v>225</v>
       </c>
       <c r="E114" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F114">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>240</v>
       </c>
@@ -4019,10 +4274,13 @@
         <v>225</v>
       </c>
       <c r="E115" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F115">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>242</v>
       </c>
@@ -4036,10 +4294,13 @@
         <v>225</v>
       </c>
       <c r="E116" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F116">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>244</v>
       </c>
@@ -4053,10 +4314,13 @@
         <v>225</v>
       </c>
       <c r="E117" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F117">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>246</v>
       </c>
@@ -4070,10 +4334,13 @@
         <v>225</v>
       </c>
       <c r="E118" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F118">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>248</v>
       </c>
@@ -4087,10 +4354,13 @@
         <v>225</v>
       </c>
       <c r="E119" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F119">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>250</v>
       </c>
@@ -4104,10 +4374,13 @@
         <v>225</v>
       </c>
       <c r="E120" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F120">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>252</v>
       </c>
@@ -4121,10 +4394,13 @@
         <v>225</v>
       </c>
       <c r="E121" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F121">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>254</v>
       </c>
@@ -4138,10 +4414,13 @@
         <v>225</v>
       </c>
       <c r="E122" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F122">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>256</v>
       </c>
@@ -4155,10 +4434,13 @@
         <v>225</v>
       </c>
       <c r="E123" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F123">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>258</v>
       </c>
@@ -4172,10 +4454,13 @@
         <v>225</v>
       </c>
       <c r="E124" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F124">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>260</v>
       </c>
@@ -4189,10 +4474,13 @@
         <v>225</v>
       </c>
       <c r="E125" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F125">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>262</v>
       </c>
@@ -4206,10 +4494,13 @@
         <v>225</v>
       </c>
       <c r="E126" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F126">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>264</v>
       </c>
@@ -4223,10 +4514,13 @@
         <v>225</v>
       </c>
       <c r="E127" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F127">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>266</v>
       </c>
@@ -4240,10 +4534,13 @@
         <v>225</v>
       </c>
       <c r="E128" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F128">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>268</v>
       </c>
@@ -4257,10 +4554,13 @@
         <v>270</v>
       </c>
       <c r="E129" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F129">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>271</v>
       </c>
@@ -4274,10 +4574,13 @@
         <v>270</v>
       </c>
       <c r="E130" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F130">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>273</v>
       </c>
@@ -4291,10 +4594,13 @@
         <v>275</v>
       </c>
       <c r="E131" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>276</v>
       </c>
@@ -4308,10 +4614,13 @@
         <v>275</v>
       </c>
       <c r="E132" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F132">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>278</v>
       </c>
@@ -4325,10 +4634,13 @@
         <v>275</v>
       </c>
       <c r="E133" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F133">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>280</v>
       </c>
@@ -4342,10 +4654,13 @@
         <v>275</v>
       </c>
       <c r="E134" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>282</v>
       </c>
@@ -4359,10 +4674,13 @@
         <v>275</v>
       </c>
       <c r="E135" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>284</v>
       </c>
@@ -4376,10 +4694,13 @@
         <v>275</v>
       </c>
       <c r="E136" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>286</v>
       </c>
@@ -4393,10 +4714,13 @@
         <v>275</v>
       </c>
       <c r="E137" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>288</v>
       </c>
@@ -4410,10 +4734,13 @@
         <v>275</v>
       </c>
       <c r="E138" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>290</v>
       </c>
@@ -4427,10 +4754,13 @@
         <v>275</v>
       </c>
       <c r="E139" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>292</v>
       </c>
@@ -4444,10 +4774,13 @@
         <v>275</v>
       </c>
       <c r="E140" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>294</v>
       </c>
@@ -4461,10 +4794,13 @@
         <v>275</v>
       </c>
       <c r="E141" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F141">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>296</v>
       </c>
@@ -4478,10 +4814,13 @@
         <v>275</v>
       </c>
       <c r="E142" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>298</v>
       </c>
@@ -4495,10 +4834,13 @@
         <v>275</v>
       </c>
       <c r="E143" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>300</v>
       </c>
@@ -4512,10 +4854,13 @@
         <v>275</v>
       </c>
       <c r="E144" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>302</v>
       </c>
@@ -4529,10 +4874,13 @@
         <v>275</v>
       </c>
       <c r="E145" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>304</v>
       </c>
@@ -4546,10 +4894,13 @@
         <v>275</v>
       </c>
       <c r="E146" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>306</v>
       </c>
@@ -4563,10 +4914,13 @@
         <v>275</v>
       </c>
       <c r="E147" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>308</v>
       </c>
@@ -4580,10 +4934,13 @@
         <v>275</v>
       </c>
       <c r="E148" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>310</v>
       </c>
@@ -4597,10 +4954,13 @@
         <v>275</v>
       </c>
       <c r="E149" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>312</v>
       </c>
@@ -4614,10 +4974,13 @@
         <v>275</v>
       </c>
       <c r="E150" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>314</v>
       </c>
@@ -4631,10 +4994,13 @@
         <v>275</v>
       </c>
       <c r="E151" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>316</v>
       </c>
@@ -4648,10 +5014,13 @@
         <v>275</v>
       </c>
       <c r="E152" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>318</v>
       </c>
@@ -4665,10 +5034,13 @@
         <v>275</v>
       </c>
       <c r="E153" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>320</v>
       </c>
@@ -4682,10 +5054,13 @@
         <v>275</v>
       </c>
       <c r="E154" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>322</v>
       </c>
@@ -4699,10 +5074,13 @@
         <v>275</v>
       </c>
       <c r="E155" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>324</v>
       </c>
@@ -4716,10 +5094,13 @@
         <v>275</v>
       </c>
       <c r="E156" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>326</v>
       </c>
@@ -4733,10 +5114,13 @@
         <v>275</v>
       </c>
       <c r="E157" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>328</v>
       </c>
@@ -4750,10 +5134,13 @@
         <v>275</v>
       </c>
       <c r="E158" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>330</v>
       </c>
@@ -4767,10 +5154,13 @@
         <v>275</v>
       </c>
       <c r="E159" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>332</v>
       </c>
@@ -4784,10 +5174,13 @@
         <v>275</v>
       </c>
       <c r="E160" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F160">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>334</v>
       </c>
@@ -4801,10 +5194,13 @@
         <v>275</v>
       </c>
       <c r="E161" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>336</v>
       </c>
@@ -4818,10 +5214,13 @@
         <v>275</v>
       </c>
       <c r="E162" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F162">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>338</v>
       </c>
@@ -4835,10 +5234,13 @@
         <v>275</v>
       </c>
       <c r="E163" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>340</v>
       </c>
@@ -4852,10 +5254,13 @@
         <v>275</v>
       </c>
       <c r="E164" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>342</v>
       </c>
@@ -4869,10 +5274,13 @@
         <v>344</v>
       </c>
       <c r="E165" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F165">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>345</v>
       </c>
@@ -4886,10 +5294,13 @@
         <v>344</v>
       </c>
       <c r="E166" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F166">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>347</v>
       </c>
@@ -4903,10 +5314,13 @@
         <v>344</v>
       </c>
       <c r="E167" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F167">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>349</v>
       </c>
@@ -4920,10 +5334,13 @@
         <v>344</v>
       </c>
       <c r="E168" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F168">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>351</v>
       </c>
@@ -4937,10 +5354,13 @@
         <v>353</v>
       </c>
       <c r="E169" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F169">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>354</v>
       </c>
@@ -4954,10 +5374,13 @@
         <v>356</v>
       </c>
       <c r="E170" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>357</v>
       </c>
@@ -4971,10 +5394,13 @@
         <v>356</v>
       </c>
       <c r="E171" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>359</v>
       </c>
@@ -4988,10 +5414,13 @@
         <v>356</v>
       </c>
       <c r="E172" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>361</v>
       </c>
@@ -5005,10 +5434,13 @@
         <v>356</v>
       </c>
       <c r="E173" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>363</v>
       </c>
@@ -5022,10 +5454,13 @@
         <v>365</v>
       </c>
       <c r="E174" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F174">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>366</v>
       </c>
@@ -5039,10 +5474,13 @@
         <v>365</v>
       </c>
       <c r="E175" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F175">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>368</v>
       </c>
@@ -5056,10 +5494,13 @@
         <v>365</v>
       </c>
       <c r="E176" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F176">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>370</v>
       </c>
@@ -5073,10 +5514,13 @@
         <v>372</v>
       </c>
       <c r="E177" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F177">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>373</v>
       </c>
@@ -5090,10 +5534,13 @@
         <v>372</v>
       </c>
       <c r="E178" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>375</v>
       </c>
@@ -5107,10 +5554,13 @@
         <v>372</v>
       </c>
       <c r="E179" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>377</v>
       </c>
@@ -5124,10 +5574,13 @@
         <v>372</v>
       </c>
       <c r="E180" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F180">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>379</v>
       </c>
@@ -5141,10 +5594,13 @@
         <v>372</v>
       </c>
       <c r="E181" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F181">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>381</v>
       </c>
@@ -5158,10 +5614,13 @@
         <v>372</v>
       </c>
       <c r="E182" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F182">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>383</v>
       </c>
@@ -5175,10 +5634,13 @@
         <v>372</v>
       </c>
       <c r="E183" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>385</v>
       </c>
@@ -5192,10 +5654,13 @@
         <v>372</v>
       </c>
       <c r="E184" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>387</v>
       </c>
@@ -5209,10 +5674,13 @@
         <v>389</v>
       </c>
       <c r="E185" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F185">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>390</v>
       </c>
@@ -5226,10 +5694,13 @@
         <v>389</v>
       </c>
       <c r="E186" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F186">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>392</v>
       </c>
@@ -5243,10 +5714,13 @@
         <v>389</v>
       </c>
       <c r="E187" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F187">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>394</v>
       </c>
@@ -5260,10 +5734,13 @@
         <v>389</v>
       </c>
       <c r="E188" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F188">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>396</v>
       </c>
@@ -5277,10 +5754,13 @@
         <v>389</v>
       </c>
       <c r="E189" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F189">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>398</v>
       </c>
@@ -5294,10 +5774,10 @@
         <v>400</v>
       </c>
       <c r="E190" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>401</v>
       </c>
@@ -5311,10 +5791,10 @@
         <v>400</v>
       </c>
       <c r="E191" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>403</v>
       </c>
@@ -5328,10 +5808,10 @@
         <v>400</v>
       </c>
       <c r="E192" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>405</v>
       </c>
@@ -5345,10 +5825,10 @@
         <v>400</v>
       </c>
       <c r="E193" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>407</v>
       </c>
@@ -5362,10 +5842,10 @@
         <v>400</v>
       </c>
       <c r="E194" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>409</v>
       </c>
@@ -5379,10 +5859,10 @@
         <v>411</v>
       </c>
       <c r="E195" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>412</v>
       </c>
@@ -5396,10 +5876,10 @@
         <v>411</v>
       </c>
       <c r="E196" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>414</v>
       </c>
@@ -5413,10 +5893,10 @@
         <v>411</v>
       </c>
       <c r="E197" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>416</v>
       </c>
@@ -5430,10 +5910,10 @@
         <v>411</v>
       </c>
       <c r="E198" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>418</v>
       </c>
@@ -5447,10 +5927,10 @@
         <v>411</v>
       </c>
       <c r="E199" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>420</v>
       </c>
@@ -5464,10 +5944,13 @@
         <v>422</v>
       </c>
       <c r="E200" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F200">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>423</v>
       </c>
@@ -5481,10 +5964,13 @@
         <v>422</v>
       </c>
       <c r="E201" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F201">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>425</v>
       </c>
@@ -5498,10 +5984,13 @@
         <v>422</v>
       </c>
       <c r="E202" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F202">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>427</v>
       </c>
@@ -5515,10 +6004,13 @@
         <v>422</v>
       </c>
       <c r="E203" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F203">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>429</v>
       </c>
@@ -5532,10 +6024,13 @@
         <v>422</v>
       </c>
       <c r="E204" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F204">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>431</v>
       </c>
@@ -5549,10 +6044,13 @@
         <v>422</v>
       </c>
       <c r="E205" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F205">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>433</v>
       </c>
@@ -5566,10 +6064,13 @@
         <v>422</v>
       </c>
       <c r="E206" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F206">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>435</v>
       </c>
@@ -5583,10 +6084,13 @@
         <v>422</v>
       </c>
       <c r="E207" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F207">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>437</v>
       </c>
@@ -5600,10 +6104,13 @@
         <v>422</v>
       </c>
       <c r="E208" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F208">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>439</v>
       </c>
@@ -5617,10 +6124,13 @@
         <v>422</v>
       </c>
       <c r="E209" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F209">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>441</v>
       </c>
@@ -5634,10 +6144,13 @@
         <v>422</v>
       </c>
       <c r="E210" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F210">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>443</v>
       </c>
@@ -5651,10 +6164,13 @@
         <v>422</v>
       </c>
       <c r="E211" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F211">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>445</v>
       </c>
@@ -5668,10 +6184,13 @@
         <v>422</v>
       </c>
       <c r="E212" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F212">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>447</v>
       </c>
@@ -5685,10 +6204,13 @@
         <v>422</v>
       </c>
       <c r="E213" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F213">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>449</v>
       </c>
@@ -5702,10 +6224,13 @@
         <v>422</v>
       </c>
       <c r="E214" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F214">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>451</v>
       </c>
@@ -5719,10 +6244,13 @@
         <v>453</v>
       </c>
       <c r="E215" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F215">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>454</v>
       </c>
@@ -5736,10 +6264,13 @@
         <v>453</v>
       </c>
       <c r="E216" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>456</v>
       </c>
@@ -5753,10 +6284,13 @@
         <v>453</v>
       </c>
       <c r="E217" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>458</v>
       </c>
@@ -5770,10 +6304,13 @@
         <v>453</v>
       </c>
       <c r="E218" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F218">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>460</v>
       </c>
@@ -5787,10 +6324,13 @@
         <v>453</v>
       </c>
       <c r="E219" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F219">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>462</v>
       </c>
@@ -5804,10 +6344,13 @@
         <v>453</v>
       </c>
       <c r="E220" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F220">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>464</v>
       </c>
@@ -5821,10 +6364,13 @@
         <v>453</v>
       </c>
       <c r="E221" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>466</v>
       </c>
@@ -5838,10 +6384,13 @@
         <v>453</v>
       </c>
       <c r="E222" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F222">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>468</v>
       </c>
@@ -5855,10 +6404,13 @@
         <v>453</v>
       </c>
       <c r="E223" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F223">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>470</v>
       </c>
@@ -5872,10 +6424,13 @@
         <v>453</v>
       </c>
       <c r="E224" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>472</v>
       </c>
@@ -5889,10 +6444,13 @@
         <v>453</v>
       </c>
       <c r="E225" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F225">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>474</v>
       </c>
@@ -5906,10 +6464,13 @@
         <v>453</v>
       </c>
       <c r="E226" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F226">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>476</v>
       </c>
@@ -5923,10 +6484,13 @@
         <v>6</v>
       </c>
       <c r="E227" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F227">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>478</v>
       </c>
@@ -5940,10 +6504,13 @@
         <v>6</v>
       </c>
       <c r="E228" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F228">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>480</v>
       </c>
@@ -5957,10 +6524,13 @@
         <v>6</v>
       </c>
       <c r="E229" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F229">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>482</v>
       </c>
@@ -5974,10 +6544,13 @@
         <v>6</v>
       </c>
       <c r="E230" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F230">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>484</v>
       </c>
@@ -5991,10 +6564,13 @@
         <v>6</v>
       </c>
       <c r="E231" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F231">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>486</v>
       </c>
@@ -6008,10 +6584,13 @@
         <v>6</v>
       </c>
       <c r="E232" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F232">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>488</v>
       </c>
@@ -6025,10 +6604,13 @@
         <v>6</v>
       </c>
       <c r="E233" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F233">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>490</v>
       </c>
@@ -6042,10 +6624,13 @@
         <v>6</v>
       </c>
       <c r="E234" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F234">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>492</v>
       </c>
@@ -6059,10 +6644,13 @@
         <v>6</v>
       </c>
       <c r="E235" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F235">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>494</v>
       </c>
@@ -6076,10 +6664,13 @@
         <v>6</v>
       </c>
       <c r="E236" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F236">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>496</v>
       </c>
@@ -6093,10 +6684,13 @@
         <v>6</v>
       </c>
       <c r="E237" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F237">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>498</v>
       </c>
@@ -6110,10 +6704,13 @@
         <v>6</v>
       </c>
       <c r="E238" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F238">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>500</v>
       </c>
@@ -6127,10 +6724,13 @@
         <v>6</v>
       </c>
       <c r="E239" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F239">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>502</v>
       </c>
@@ -6144,10 +6744,13 @@
         <v>6</v>
       </c>
       <c r="E240" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F240">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>504</v>
       </c>
@@ -6161,10 +6764,13 @@
         <v>6</v>
       </c>
       <c r="E241" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F241">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>506</v>
       </c>
@@ -6178,10 +6784,13 @@
         <v>6</v>
       </c>
       <c r="E242" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F242">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>508</v>
       </c>
@@ -6195,10 +6804,13 @@
         <v>6</v>
       </c>
       <c r="E243" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F243">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>510</v>
       </c>
@@ -6212,10 +6824,13 @@
         <v>6</v>
       </c>
       <c r="E244" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F244">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>512</v>
       </c>
@@ -6229,10 +6844,13 @@
         <v>6</v>
       </c>
       <c r="E245" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F245">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>514</v>
       </c>
@@ -6246,10 +6864,13 @@
         <v>6</v>
       </c>
       <c r="E246" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F246">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>516</v>
       </c>
@@ -6263,10 +6884,13 @@
         <v>6</v>
       </c>
       <c r="E247" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F247">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>518</v>
       </c>
@@ -6280,10 +6904,13 @@
         <v>6</v>
       </c>
       <c r="E248" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F248">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>520</v>
       </c>
@@ -6297,10 +6924,13 @@
         <v>6</v>
       </c>
       <c r="E249" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F249">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>522</v>
       </c>
@@ -6314,10 +6944,13 @@
         <v>6</v>
       </c>
       <c r="E250" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="F250">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>524</v>
       </c>
@@ -6331,7 +6964,10 @@
         <v>6</v>
       </c>
       <c r="E251" t="s">
-        <v>527</v>
+        <v>526</v>
+      </c>
+      <c r="F251">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>